<commit_message>
before changing the project structure
</commit_message>
<xml_diff>
--- a/build/resources/main/Data.xlsx
+++ b/build/resources/main/Data.xlsx
@@ -3,23 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Projects\build out\Finology\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94C23D1-FA01-4958-8947-3E49B364C6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33028B3B-C560-4260-A6AB-CC161DEFEA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUpPage" sheetId="3" r:id="rId1"/>
     <sheet name="LoginPage" sheetId="1" r:id="rId2"/>
     <sheet name="HomePage" sheetId="2" r:id="rId3"/>
+    <sheet name="Login Mobile Number" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>You already have an account. Please Login to continue.</t>
   </si>
@@ -62,9 +63,6 @@
     <t>Invalid Email</t>
   </si>
   <si>
-    <t xml:space="preserve">$Lakesh Sahu, </t>
-  </si>
-  <si>
     <t>empty name</t>
   </si>
   <si>
@@ -84,12 +82,76 @@
   </si>
   <si>
     <t>invalid mobile number, 123456789, @@@@@$#@$#</t>
+  </si>
+  <si>
+    <t>invalidEmail</t>
+  </si>
+  <si>
+    <t>empty email</t>
+  </si>
+  <si>
+    <t>Locator</t>
+  </si>
+  <si>
+    <t>id = "txtCustomerName-error"</t>
+  </si>
+  <si>
+    <t>id = "spanName"</t>
+  </si>
+  <si>
+    <t>emptyName</t>
+  </si>
+  <si>
+    <t>id = "Email-error"</t>
+  </si>
+  <si>
+    <t>$Lakesh Sahu, TestUser124</t>
+  </si>
+  <si>
+    <t>login mobile number</t>
+  </si>
+  <si>
+    <t>6719398636</t>
+  </si>
+  <si>
+    <t>6122843982</t>
+  </si>
+  <si>
+    <t>5116969645</t>
+  </si>
+  <si>
+    <t>2201481203</t>
+  </si>
+  <si>
+    <t>8718797752</t>
+  </si>
+  <si>
+    <t>8857645320</t>
+  </si>
+  <si>
+    <t>9147575039</t>
+  </si>
+  <si>
+    <t>7302560739</t>
+  </si>
+  <si>
+    <t>3616666007</t>
+  </si>
+  <si>
+    <t>3136865597</t>
+  </si>
+  <si>
+    <t>5917790642</t>
+  </si>
+  <si>
+    <t>1786814810</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -412,80 +474,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5CF1B9-8E45-4D3F-9539-0C418DE474C4}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="73.88671875" customWidth="1"/>
-    <col min="3" max="3" width="77.5546875" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.33203125"/>
+    <col min="2" max="2" customWidth="true" width="51.44140625"/>
+    <col min="3" max="3" customWidth="true" width="53.33203125"/>
+    <col min="4" max="4" customWidth="true" width="27.21875"/>
+    <col min="5" max="5" customWidth="true" width="44.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D1" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="D3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D5" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s" s="0">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C7" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s" s="0">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+      <c r="E9" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s" s="0">
         <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -505,20 +594,24 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="28.5546875"/>
+    <col min="2" max="2" customWidth="true" width="47.6640625"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>0</v>
       </c>
     </row>
@@ -537,4 +630,87 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBA4F1F-B5DD-4869-9E5A-AFDBC028E53A}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="28.33203125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update scenario status excel report
</commit_message>
<xml_diff>
--- a/build/resources/main/Data.xlsx
+++ b/build/resources/main/Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
   <si>
     <t>You already have an account. Please Login to continue.</t>
   </si>
@@ -190,6 +190,273 @@
   </si>
   <si>
     <t>9820207251</t>
+  </si>
+  <si>
+    <t>9481758105</t>
+  </si>
+  <si>
+    <t>2718454523</t>
+  </si>
+  <si>
+    <t>2154478176</t>
+  </si>
+  <si>
+    <t>3728940729</t>
+  </si>
+  <si>
+    <t>7261910232</t>
+  </si>
+  <si>
+    <t>8105886786</t>
+  </si>
+  <si>
+    <t>8647284553</t>
+  </si>
+  <si>
+    <t>5373968912</t>
+  </si>
+  <si>
+    <t>4131060765</t>
+  </si>
+  <si>
+    <t>4087557155</t>
+  </si>
+  <si>
+    <t>6582291831</t>
+  </si>
+  <si>
+    <t>4956187639</t>
+  </si>
+  <si>
+    <t>1604155166</t>
+  </si>
+  <si>
+    <t>4445460072</t>
+  </si>
+  <si>
+    <t>0120437413</t>
+  </si>
+  <si>
+    <t>1984094441</t>
+  </si>
+  <si>
+    <t>8372006150</t>
+  </si>
+  <si>
+    <t>9737934498</t>
+  </si>
+  <si>
+    <t>4462166045</t>
+  </si>
+  <si>
+    <t>7472031041</t>
+  </si>
+  <si>
+    <t>2272891346</t>
+  </si>
+  <si>
+    <t>4764757375</t>
+  </si>
+  <si>
+    <t>9618079294</t>
+  </si>
+  <si>
+    <t>6746417643</t>
+  </si>
+  <si>
+    <t>6358885530</t>
+  </si>
+  <si>
+    <t>3942262542</t>
+  </si>
+  <si>
+    <t>5829839274</t>
+  </si>
+  <si>
+    <t>2464542431</t>
+  </si>
+  <si>
+    <t>4936201314</t>
+  </si>
+  <si>
+    <t>7521146830</t>
+  </si>
+  <si>
+    <t>1031496065</t>
+  </si>
+  <si>
+    <t>3822327461</t>
+  </si>
+  <si>
+    <t>9559405562</t>
+  </si>
+  <si>
+    <t>3040277876</t>
+  </si>
+  <si>
+    <t>7514424092</t>
+  </si>
+  <si>
+    <t>6770262251</t>
+  </si>
+  <si>
+    <t>0939873681</t>
+  </si>
+  <si>
+    <t>8356831008</t>
+  </si>
+  <si>
+    <t>9294548500</t>
+  </si>
+  <si>
+    <t>2752916912</t>
+  </si>
+  <si>
+    <t>3573140489</t>
+  </si>
+  <si>
+    <t>5768779175</t>
+  </si>
+  <si>
+    <t>6263099966</t>
+  </si>
+  <si>
+    <t>1852755047</t>
+  </si>
+  <si>
+    <t>2787555746</t>
+  </si>
+  <si>
+    <t>8637837862</t>
+  </si>
+  <si>
+    <t>6517517021</t>
+  </si>
+  <si>
+    <t>5826411890</t>
+  </si>
+  <si>
+    <t>9712625243</t>
+  </si>
+  <si>
+    <t>2023262132</t>
+  </si>
+  <si>
+    <t>9803240222</t>
+  </si>
+  <si>
+    <t>9965146585</t>
+  </si>
+  <si>
+    <t>9141897296</t>
+  </si>
+  <si>
+    <t>4539727291</t>
+  </si>
+  <si>
+    <t>2264992038</t>
+  </si>
+  <si>
+    <t>4688608568</t>
+  </si>
+  <si>
+    <t>2042397159</t>
+  </si>
+  <si>
+    <t>1740477750</t>
+  </si>
+  <si>
+    <t>8331408592</t>
+  </si>
+  <si>
+    <t>0519256949</t>
+  </si>
+  <si>
+    <t>6987426695</t>
+  </si>
+  <si>
+    <t>8455189902</t>
+  </si>
+  <si>
+    <t>1934961017</t>
+  </si>
+  <si>
+    <t>5104174812</t>
+  </si>
+  <si>
+    <t>1919940069</t>
+  </si>
+  <si>
+    <t>3919811534</t>
+  </si>
+  <si>
+    <t>2924347501</t>
+  </si>
+  <si>
+    <t>1452040359</t>
+  </si>
+  <si>
+    <t>4902488420</t>
+  </si>
+  <si>
+    <t>9388864286</t>
+  </si>
+  <si>
+    <t>9057072236</t>
+  </si>
+  <si>
+    <t>9798538334</t>
+  </si>
+  <si>
+    <t>1351428444</t>
+  </si>
+  <si>
+    <t>1036775979</t>
+  </si>
+  <si>
+    <t>4571959374</t>
+  </si>
+  <si>
+    <t>1059585427</t>
+  </si>
+  <si>
+    <t>9100554479</t>
+  </si>
+  <si>
+    <t>3674500568</t>
+  </si>
+  <si>
+    <t>6118490504</t>
+  </si>
+  <si>
+    <t>7391918471</t>
+  </si>
+  <si>
+    <t>2221750282</t>
+  </si>
+  <si>
+    <t>3033728593</t>
+  </si>
+  <si>
+    <t>0107710010</t>
+  </si>
+  <si>
+    <t>3302772706</t>
+  </si>
+  <si>
+    <t>7581740116</t>
+  </si>
+  <si>
+    <t>4711103563</t>
+  </si>
+  <si>
+    <t>6351813634</t>
+  </si>
+  <si>
+    <t>3926414576</t>
+  </si>
+  <si>
+    <t>4845749618</t>
   </si>
 </sst>
 </file>
@@ -679,7 +946,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBA4F1F-B5DD-4869-9E5A-AFDBC028E53A}">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -830,6 +1097,451 @@
         <v>53</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="0">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="0">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="0">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="0">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="0">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="0">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="0">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="0">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="0">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="0">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="0">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="0">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="0">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="0">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="0">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="0">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="0">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="0">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="0">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="0">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="0">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="0">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="0">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="0">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="0">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="0">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="0">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="0">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="0">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="0">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="0">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="0">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="0">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="0">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="0">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="0">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="0">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="0">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="0">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="0">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="0">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="0">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="0">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>